<commit_message>
unit test with bug fix
</commit_message>
<xml_diff>
--- a/Course_Plan.xlsx
+++ b/Course_Plan.xlsx
@@ -62,13 +62,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,7 +452,7 @@
     <col width="40" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" ht="30" customHeight="1">
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Study Plan</t>
@@ -489,12 +489,12 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>CPSC 6179</t>
+          <t>CPSC 6127</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Software Project Planning and Management</t>
+          <t>Contemporary Issues in Database Management Systems</t>
         </is>
       </c>
     </row>
@@ -511,22 +511,22 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>CPSC 6127</t>
+          <t>CPSC 6179</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Contemporary Issues in Database Management Systems</t>
+          <t>Software Project Planning and Management</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="2" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>CPSC 6000</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>Graduate Exit Examination in Computer Science</t>
         </is>
@@ -535,12 +535,12 @@
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
         <is>
+          <t>Courses: 2</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
           <t>Courses: 3</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>Courses: 2</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">

</xml_diff>